<commit_message>
Added the add doc item form, need to improve
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D1BF5DD-DCA6-4360-88CD-A920774B16DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D2CD96-03D6-4AF8-B2D9-FD31553C3722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +460,9 @@
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working on the add new document form
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D2CD96-03D6-4AF8-B2D9-FD31553C3722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26393EDD-9CBF-41C7-A8C4-AD7AC95EC4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>add item form</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>Original cost</t>
+  </si>
+  <si>
+    <t>product_cost</t>
+  </si>
+  <si>
+    <t>price_before_tax</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>product_margin</t>
+  </si>
+  <si>
+    <t>base_price</t>
+  </si>
+  <si>
+    <t>per item</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -449,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9502E6FF-377B-4B1C-ADE1-A65815E2CFDF}">
-  <dimension ref="B1:E6"/>
+  <dimension ref="B1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +558,87 @@
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>183.75</v>
+      </c>
+      <c r="E26">
+        <v>0.05</v>
+      </c>
+      <c r="F26">
+        <f>D26+(D26*E26)</f>
+        <v>192.9375</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
drew some guidline to create an order
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26393EDD-9CBF-41C7-A8C4-AD7AC95EC4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9E0104-6A2D-489E-B070-9F10317A54CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>add item form</t>
   </si>
@@ -80,28 +80,31 @@
     <t>Original cost</t>
   </si>
   <si>
-    <t>product_cost</t>
-  </si>
-  <si>
-    <t>price_before_tax</t>
-  </si>
-  <si>
-    <t>tax</t>
-  </si>
-  <si>
-    <t>discount</t>
-  </si>
-  <si>
-    <t>product_margin</t>
-  </si>
-  <si>
-    <t>base_price</t>
-  </si>
-  <si>
-    <t>per item</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>Necessary payload:</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Nnumber</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Cash register</t>
   </si>
 </sst>
 </file>
@@ -117,12 +120,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,8 +146,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,23 +483,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9502E6FF-377B-4B1C-ADE1-A65815E2CFDF}">
-  <dimension ref="B1:F27"/>
+  <dimension ref="B1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" customWidth="1"/>
     <col min="7" max="7" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -500,7 +510,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -514,7 +524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -522,7 +532,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -530,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -544,7 +554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -558,85 +568,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>183.75</v>
-      </c>
-      <c r="E26">
-        <v>0.05</v>
-      </c>
-      <c r="F26">
-        <f>D26+(D26*E26)</f>
-        <v>192.9375</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E27" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on template for the documents
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\hud\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9E0104-6A2D-489E-B070-9F10317A54CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3172AB-8536-442E-8C21-9848E373DD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
   <si>
     <t>add item form</t>
   </si>
@@ -105,13 +105,153 @@
   </si>
   <si>
     <t>Cash register</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>refund</t>
+  </si>
+  <si>
+    <t>stock_return</t>
+  </si>
+  <si>
+    <t>proforma</t>
+  </si>
+  <si>
+    <t>expenses</t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>loss_and_damage</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>due_date</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>discounts</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>stock_date</t>
+  </si>
+  <si>
+    <t>external_document</t>
+  </si>
+  <si>
+    <t>internal_note</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>FORM</t>
+  </si>
+  <si>
+    <t>INITIALS</t>
+  </si>
+  <si>
+    <t>{doc_type}-randint'</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>From_setting</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>REQUIRED</t>
+  </si>
+  <si>
+    <t>REQUIRED_VALUES</t>
+  </si>
+  <si>
+    <t>document_type</t>
+  </si>
+  <si>
+    <t>1. How many was available</t>
+  </si>
+  <si>
+    <t>2. How many have been sold</t>
+  </si>
+  <si>
+    <t>3. What was the price then</t>
+  </si>
+  <si>
+    <t>4. General condition of the product</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Inventory count:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> counts the count of products in the stock to show the status of a product at a certain date:</t>
+    </r>
+  </si>
+  <si>
+    <t>inventory_count *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,8 +259,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,8 +288,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -142,13 +327,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,128 +704,585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9502E6FF-377B-4B1C-ADE1-A65815E2CFDF}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="3" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="I6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+      <c r="C27" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s">
+        <v>38</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s">
+        <v>39</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="K34" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K38" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost fixed the document form, needs doc item form
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3172AB-8536-442E-8C21-9848E373DD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDE4AED-EB70-4D84-B0A1-79D09A616242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Document" sheetId="1" r:id="rId1"/>
+    <sheet name="items" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="77">
   <si>
     <t>add item form</t>
   </si>
@@ -246,12 +247,57 @@
   <si>
     <t>inventory_count *</t>
   </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>expected_quantity</t>
+  </si>
+  <si>
+    <t>price_before_tax</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>discount_type</t>
+  </si>
+  <si>
+    <t>product_cost</t>
+  </si>
+  <si>
+    <t>price_after_discount</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>total_after_document_discount</t>
+  </si>
+  <si>
+    <t>discount_apply_rule</t>
+  </si>
+  <si>
+    <t>price_before_tax_aafter_discount</t>
+  </si>
+  <si>
+    <t>returned</t>
+  </si>
+  <si>
+    <t>product.price</t>
+  </si>
+  <si>
+    <t>product.price * quantity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +319,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -351,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -367,9 +418,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9502E6FF-377B-4B1C-ADE1-A65815E2CFDF}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,4 +1342,550 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBA61CF-EB0F-4A59-80F4-96CD30CD112F}">
+  <dimension ref="A1:M42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+    </row>
+    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+    </row>
+    <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+    </row>
+    <row r="25" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+    </row>
+    <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+    </row>
+    <row r="27" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+    </row>
+    <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+    </row>
+    <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+    </row>
+    <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+    </row>
+    <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+    </row>
+    <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+    </row>
+    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+    </row>
+    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+    </row>
+    <row r="35" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+    </row>
+    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+    </row>
+    <row r="37" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+    </row>
+    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+    </row>
+    <row r="39" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+    </row>
+    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+    </row>
+    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+    </row>
+    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the orders, now time to create one
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDE4AED-EB70-4D84-B0A1-79D09A616242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F635A4D6-7A9A-4313-B009-DD1A6B2BB3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="81">
   <si>
     <t>add item form</t>
   </si>
@@ -292,12 +292,24 @@
   <si>
     <t>product.price * quantity</t>
   </si>
+  <si>
+    <t>add new document</t>
+  </si>
+  <si>
+    <t>if already created</t>
+  </si>
+  <si>
+    <t>if add new</t>
+  </si>
+  <si>
+    <t>select_document</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,7 +776,7 @@
       <selection activeCell="C38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -779,7 +791,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:10">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="6:10">
       <c r="F2">
         <v>1</v>
       </c>
@@ -804,7 +816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:10">
       <c r="F3">
         <v>2</v>
       </c>
@@ -812,7 +824,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:10">
       <c r="F4">
         <v>3</v>
       </c>
@@ -820,7 +832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:10">
       <c r="F5">
         <v>4</v>
       </c>
@@ -834,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:10">
       <c r="F6">
         <v>5</v>
       </c>
@@ -848,12 +860,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:10">
       <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:10">
       <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
@@ -867,27 +879,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:10">
       <c r="H13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:10">
       <c r="H14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:10">
       <c r="H15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:10">
       <c r="H16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
@@ -901,7 +913,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -937,7 +949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -973,7 +985,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1007,7 +1019,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1041,7 +1053,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1112,7 +1124,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1146,7 +1158,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1180,7 +1192,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1214,7 +1226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1248,7 +1260,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1276,7 +1288,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1295,7 +1307,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1314,27 +1326,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="60">
       <c r="K34" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="K35" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="K36" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="K37" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="30">
       <c r="K38" s="7" t="s">
         <v>59</v>
       </c>
@@ -1349,10 +1361,10 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -1367,7 +1379,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1381,7 +1393,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1417,7 +1429,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1453,7 +1465,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1487,7 +1499,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1523,7 +1535,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1560,7 +1572,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1594,7 +1606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1630,7 +1642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1666,7 +1678,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1700,7 +1712,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1734,7 +1746,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1783,7 +1795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1802,87 +1814,99 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="16.5">
       <c r="A22" s="12"/>
     </row>
-    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="16.5">
       <c r="A23" s="12"/>
     </row>
-    <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="16.5">
       <c r="A24" s="12"/>
     </row>
-    <row r="25" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-    </row>
-    <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-    </row>
-    <row r="27" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-    </row>
-    <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.5">
+      <c r="A25" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16.5">
+      <c r="A26" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16.5">
+      <c r="A27" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16.5">
       <c r="A28" s="12"/>
     </row>
-    <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="16.5">
       <c r="A29" s="12"/>
     </row>
-    <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="16.5">
       <c r="A30" s="12"/>
     </row>
-    <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="16.5">
       <c r="A31" s="12"/>
     </row>
-    <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="16.5">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="16.5">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="16.5">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="16.5">
       <c r="A35" s="12"/>
     </row>
-    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" ht="16.5">
       <c r="A36" s="12"/>
     </row>
-    <row r="37" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="12"/>
     </row>
-    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="12"/>
     </row>
-    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the add new doc, now need to fix the table rendering
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\hud\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F635A4D6-7A9A-4313-B009-DD1A6B2BB3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00031A3D-D506-47FF-8B2D-B57454F946A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="84">
   <si>
     <t>add item form</t>
   </si>
@@ -304,12 +304,21 @@
   <si>
     <t>select_document</t>
   </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>new 1</t>
+  </si>
+  <si>
+    <t>new 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -776,7 +785,7 @@
       <selection activeCell="C38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -791,7 +800,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:10">
+    <row r="1" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="6:10">
+    <row r="2" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>1</v>
       </c>
@@ -816,7 +825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="6:10">
+    <row r="3" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F3">
         <v>2</v>
       </c>
@@ -824,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="6:10">
+    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>3</v>
       </c>
@@ -832,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="6:10">
+    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>4</v>
       </c>
@@ -846,7 +855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="6:10">
+    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>5</v>
       </c>
@@ -860,12 +869,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="6:10">
+    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="6:10">
+    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
       <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
@@ -879,27 +888,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="6:10">
+    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="6:10">
+    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="6:10">
+    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="6:10">
+    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
@@ -913,7 +922,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -949,7 +958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -985,7 +994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1028,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1192,7 +1201,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1260,7 +1269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1288,7 +1297,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1307,7 +1316,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1326,27 +1335,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="60">
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="K34" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K35" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K36" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K37" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30">
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="K38" s="7" t="s">
         <v>59</v>
       </c>
@@ -1361,10 +1370,10 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -1379,7 +1388,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1429,7 +1438,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1465,7 +1474,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1535,7 +1544,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1572,7 +1581,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1606,7 +1615,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1642,7 +1651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1746,7 +1755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1776,7 +1785,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1814,41 +1823,41 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.5">
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
     </row>
-    <row r="23" spans="1:2" ht="16.5">
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
     </row>
-    <row r="24" spans="1:2" ht="16.5">
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
     </row>
-    <row r="25" spans="1:2" ht="16.5">
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.5">
+    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>78</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.5">
+    <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>79</v>
       </c>
@@ -1864,49 +1873,61 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.5">
+    <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
     </row>
-    <row r="29" spans="1:2" ht="16.5">
+    <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
-    </row>
-    <row r="30" spans="1:2" ht="16.5">
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
-    </row>
-    <row r="31" spans="1:2" ht="16.5">
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
     </row>
-    <row r="32" spans="1:2" ht="16.5">
+    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:1" ht="16.5">
+    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:1" ht="16.5">
+    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:1" ht="16.5">
+    <row r="35" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
     </row>
-    <row r="36" spans="1:1" ht="16.5">
+    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc item fixed, now to save document and remove order with its items
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00031A3D-D506-47FF-8B2D-B57454F946A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03114BF6-74BD-4ABE-B385-FEF7B958A461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
-    <sheet name="items" sheetId="2" r:id="rId2"/>
+    <sheet name="document_items" sheetId="2" r:id="rId2"/>
+    <sheet name="order_item" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="133">
   <si>
     <t>add item form</t>
   </si>
@@ -312,6 +313,153 @@
   </si>
   <si>
     <t>new 2</t>
+  </si>
+  <si>
+    <t>class PosOrderItem(models.Model):</t>
+  </si>
+  <si>
+    <t>number = models.CharField(</t>
+  </si>
+  <si>
+    <t>max_length=100, primary_key=True, db_index=True, unique=True)</t>
+  </si>
+  <si>
+    <t>user = models.ForeignKey(</t>
+  </si>
+  <si>
+    <t>User, on_delete=models.CASCADE, related_name="order_items"</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>order = models.ForeignKey(</t>
+  </si>
+  <si>
+    <t>"PosOrder", on_delete=models.CASCADE, null=True, related_name="items"</t>
+  </si>
+  <si>
+    <t>product = models.ForeignKey(</t>
+  </si>
+  <si>
+    <t>Product, on_delete=models.DO_NOTHING, related_name="order_items"</t>
+  </si>
+  <si>
+    <t>round_number = models.DecimalField(</t>
+  </si>
+  <si>
+    <t>decimal_places=3, max_digits=4, default=0)</t>
+  </si>
+  <si>
+    <t>quantity = models.IntegerField(default=1)</t>
+  </si>
+  <si>
+    <t>price = models.DecimalField(decimal_places=3,  max_digits=15, default=0)</t>
+  </si>
+  <si>
+    <t>is_locked = models.BooleanField(default=False)</t>
+  </si>
+  <si>
+    <t>discount = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>discount_type = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>is_featured = models.BooleanField(default=False)</t>
+  </si>
+  <si>
+    <t>voided_by = models.SmallIntegerField(default=0)</t>
+  </si>
+  <si>
+    <t>comment = models.TextField(null=True, blank=True)</t>
+  </si>
+  <si>
+    <t>bundle = models.TextField(null=True, blank=True)</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>round_number</t>
+  </si>
+  <si>
+    <t>bundle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">discount </t>
+  </si>
+  <si>
+    <t>is_featured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">voided_by </t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>class DocumentItem(models.Model):</t>
+  </si>
+  <si>
+    <t># number = models.UUIDField(default=uuid_lib.uuid4,</t>
+  </si>
+  <si>
+    <t>#   unique=True, primary_key=True)</t>
+  </si>
+  <si>
+    <t>User, on_delete=models.CASCADE,</t>
+  </si>
+  <si>
+    <t>related_name="document_items"</t>
+  </si>
+  <si>
+    <t>document = models.ForeignKey(</t>
+  </si>
+  <si>
+    <t>"Document", on_delete=models.CASCADE, null=True, related_name="document_items"</t>
+  </si>
+  <si>
+    <t>Product, on_delete=models.DO_NOTHING, related_name="document_items"</t>
+  </si>
+  <si>
+    <t>quantity = models.SmallIntegerField(default=1)</t>
+  </si>
+  <si>
+    <t>expected_quantity = models.SmallIntegerField(default=1)</t>
+  </si>
+  <si>
+    <t>price_before_tax = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>price = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>product_cost = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>price_before_tax_after_discount = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>price_after_discount = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>total = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>total_after_document_discount = models.FloatField(default=0)</t>
+  </si>
+  <si>
+    <t>discount_apply_rule = models.SmallIntegerField(default=0)</t>
+  </si>
+  <si>
+    <t>returned = models.BooleanField(default=False)</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBA61CF-EB0F-4A59-80F4-96CD30CD112F}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,4 +2081,257 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9588597D-AD67-4077-BADC-DBF8238ACB11}">
+  <dimension ref="A2:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" t="s">
+        <v>105</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="N9" t="s">
+        <v>106</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N10" t="s">
+        <v>63</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" t="s">
+        <v>107</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="N12" t="s">
+        <v>109</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" t="s">
+        <v>110</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="N15" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16" t="s">
+        <v>111</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N17" t="s">
+        <v>112</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" t="s">
+        <v>113</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="N19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="P25" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="P26" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="P27" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaning up the tree and rearranging all templates in place
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03114BF6-74BD-4ABE-B385-FEF7B958A461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D913BF-4420-40C6-A7A6-7AD663DA8A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="1950" yWindow="285" windowWidth="26715" windowHeight="15315" activeTab="3" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
     <sheet name="document_items" sheetId="2" r:id="rId2"/>
     <sheet name="order_item" sheetId="3" r:id="rId3"/>
+    <sheet name="Tree" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="142">
   <si>
     <t>add item form</t>
   </si>
@@ -461,12 +462,39 @@
   <si>
     <t>returned = models.BooleanField(default=False)</t>
   </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>documents</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>management</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,7 +599,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -592,6 +620,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -933,7 +964,7 @@
       <selection activeCell="C38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -948,7 +979,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:10">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="6:10">
       <c r="F2">
         <v>1</v>
       </c>
@@ -973,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:10">
       <c r="F3">
         <v>2</v>
       </c>
@@ -981,7 +1012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:10">
       <c r="F4">
         <v>3</v>
       </c>
@@ -989,7 +1020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:10">
       <c r="F5">
         <v>4</v>
       </c>
@@ -1003,7 +1034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:10">
       <c r="F6">
         <v>5</v>
       </c>
@@ -1017,12 +1048,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:10">
       <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:10">
       <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1036,27 +1067,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:10">
       <c r="H13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:10">
       <c r="H14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:10">
       <c r="H15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:10">
       <c r="H16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1070,7 +1101,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1106,7 +1137,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1142,7 +1173,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1176,7 +1207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1210,7 +1241,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1247,7 +1278,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1281,7 +1312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1315,7 +1346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1349,7 +1380,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1383,7 +1414,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1417,7 +1448,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1445,7 +1476,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1464,7 +1495,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1483,27 +1514,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="60">
       <c r="K34" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="K35" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="K36" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="K37" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="30">
       <c r="K38" s="7" t="s">
         <v>59</v>
       </c>
@@ -1521,7 +1552,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -1536,7 +1567,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1550,7 +1581,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1586,7 +1617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1622,7 +1653,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1656,7 +1687,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1692,7 +1723,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1729,7 +1760,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1763,7 +1794,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1799,7 +1830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1835,7 +1866,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1869,7 +1900,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1903,7 +1934,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1933,7 +1964,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1952,7 +1983,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1971,41 +2002,41 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16.5">
       <c r="A22" s="12"/>
     </row>
-    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16.5">
       <c r="A23" s="12"/>
     </row>
-    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16.5">
       <c r="A24" s="12"/>
     </row>
-    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16.5">
       <c r="A25" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="16.5">
       <c r="A26" s="12" t="s">
         <v>78</v>
       </c>
@@ -2013,7 +2044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="16.5">
       <c r="A27" s="12" t="s">
         <v>79</v>
       </c>
@@ -2021,10 +2052,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16.5">
       <c r="A28" s="12"/>
     </row>
-    <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="16.5">
       <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>81</v>
@@ -2036,46 +2067,46 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="16.5">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="16.5">
       <c r="A31" s="12"/>
     </row>
-    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="16.5">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="16.5">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="16.5">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="16.5">
       <c r="A35" s="12"/>
     </row>
-    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="12"/>
     </row>
-    <row r="37" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="12"/>
     </row>
-    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" s="12"/>
     </row>
-    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="12"/>
     </row>
   </sheetData>
@@ -2087,13 +2118,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9588597D-AD67-4077-BADC-DBF8238ACB11}">
   <dimension ref="A2:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="16.5">
       <c r="A2" s="12" t="s">
         <v>84</v>
       </c>
@@ -2101,7 +2132,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="16.5">
       <c r="A3" s="12" t="s">
         <v>85</v>
       </c>
@@ -2109,7 +2140,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="12" t="s">
         <v>86</v>
       </c>
@@ -2117,7 +2148,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="16.5">
       <c r="A5" s="12" t="s">
         <v>87</v>
       </c>
@@ -2125,7 +2156,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="16.5">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -2133,7 +2164,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="16.5">
       <c r="A7" s="12" t="s">
         <v>89</v>
       </c>
@@ -2144,7 +2175,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="16.5">
       <c r="A8" s="12" t="s">
         <v>90</v>
       </c>
@@ -2155,7 +2186,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="16.5">
       <c r="A9" s="12" t="s">
         <v>91</v>
       </c>
@@ -2166,7 +2197,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="16.5">
       <c r="A10" s="12" t="s">
         <v>89</v>
       </c>
@@ -2177,7 +2208,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="16.5">
       <c r="A11" s="12" t="s">
         <v>92</v>
       </c>
@@ -2188,7 +2219,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="16.5">
       <c r="A12" s="12" t="s">
         <v>93</v>
       </c>
@@ -2199,7 +2230,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="16.5">
       <c r="A13" s="12" t="s">
         <v>89</v>
       </c>
@@ -2210,7 +2241,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="16.5">
       <c r="A14" s="12" t="s">
         <v>94</v>
       </c>
@@ -2221,7 +2252,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="16.5">
       <c r="A15" s="12" t="s">
         <v>95</v>
       </c>
@@ -2232,7 +2263,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="16.5">
       <c r="A16" s="12" t="s">
         <v>96</v>
       </c>
@@ -2243,7 +2274,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="12" t="s">
         <v>97</v>
       </c>
@@ -2254,7 +2285,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="16.5">
       <c r="A18" s="12" t="s">
         <v>98</v>
       </c>
@@ -2265,7 +2296,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="16.5">
       <c r="A19" s="12" t="s">
         <v>99</v>
       </c>
@@ -2276,7 +2307,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="16.5">
       <c r="A20" s="12" t="s">
         <v>100</v>
       </c>
@@ -2284,7 +2315,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="16.5">
       <c r="A21" s="12" t="s">
         <v>101</v>
       </c>
@@ -2292,7 +2323,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="16.5">
       <c r="A22" s="12" t="s">
         <v>102</v>
       </c>
@@ -2300,7 +2331,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="16.5">
       <c r="A23" s="12" t="s">
         <v>103</v>
       </c>
@@ -2308,7 +2339,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="16.5">
       <c r="A24" s="12" t="s">
         <v>104</v>
       </c>
@@ -2316,19 +2347,107 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="16.5">
       <c r="P25" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="16.5">
       <c r="P26" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="16.5">
       <c r="P27" s="12" t="s">
         <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38477F8-6359-40BD-9417-44E5736CB004}">
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="13"/>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="13"/>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Need to calculate all the functions I have
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D913BF-4420-40C6-A7A6-7AD663DA8A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D1A0C-0710-475B-9FA8-9E0F73DCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="285" windowWidth="26715" windowHeight="15315" activeTab="3" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26715" windowHeight="15315" activeTab="4" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
     <sheet name="document_items" sheetId="2" r:id="rId2"/>
     <sheet name="order_item" sheetId="3" r:id="rId3"/>
     <sheet name="Tree" sheetId="4" r:id="rId4"/>
+    <sheet name="Views" sheetId="5" r:id="rId5"/>
+    <sheet name="temp" sheetId="7" r:id="rId6"/>
+    <sheet name="Options" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="186">
   <si>
     <t>add item form</t>
   </si>
@@ -489,12 +492,144 @@
   <si>
     <t>edit</t>
   </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>mgt_products</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t>mgt_modals</t>
+  </si>
+  <si>
+    <t>mgt_documents</t>
+  </si>
+  <si>
+    <t>mgt_document_items</t>
+  </si>
+  <si>
+    <t>modal_add_product</t>
+  </si>
+  <si>
+    <t>add_to_product_tax_formset</t>
+  </si>
+  <si>
+    <t>delete_product_tax</t>
+  </si>
+  <si>
+    <t>modal_delete_product</t>
+  </si>
+  <si>
+    <t>modal_update_product_group</t>
+  </si>
+  <si>
+    <t>modal_add_product_group</t>
+  </si>
+  <si>
+    <t>modal_delete_product_group</t>
+  </si>
+  <si>
+    <t>show_customer_form</t>
+  </si>
+  <si>
+    <t>append_product_tax_form</t>
+  </si>
+  <si>
+    <t>generate_barcode_for_product</t>
+  </si>
+  <si>
+    <t>select_product_fields_to_export</t>
+  </si>
+  <si>
+    <t>modal_add_document</t>
+  </si>
+  <si>
+    <t>modal_select_document_type</t>
+  </si>
+  <si>
+    <t>add_new_document_tab</t>
+  </si>
+  <si>
+    <t>filter_document_type</t>
+  </si>
+  <si>
+    <t>add_new_document_product_details</t>
+  </si>
+  <si>
+    <t>modal_delete_order_item</t>
+  </si>
+  <si>
+    <t>add_new_document_edit_item</t>
+  </si>
+  <si>
+    <t>DocumentSerializer</t>
+  </si>
+  <si>
+    <t>ItemListView</t>
+  </si>
+  <si>
+    <t>get_document_data</t>
+  </si>
+  <si>
+    <t>mgt_documents_example</t>
+  </si>
+  <si>
+    <t>create_order_dict</t>
+  </si>
+  <si>
+    <t>mgt_add_new_order</t>
+  </si>
+  <si>
+    <t>add_document</t>
+  </si>
+  <si>
+    <t>documents_datatable_view2</t>
+  </si>
+  <si>
+    <t>mgt_documents2</t>
+  </si>
+  <si>
+    <t>add_document_items_to_document</t>
+  </si>
+  <si>
+    <t>add_document_remove_items</t>
+  </si>
+  <si>
+    <t>add_document_change_qty</t>
+  </si>
+  <si>
+    <t>DocumentListView</t>
+  </si>
+  <si>
+    <t>get_document_dict</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +655,17 @@
     <font>
       <sz val="11"/>
       <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -599,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -624,6 +770,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,6 +791,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{071852ED-39C9-45C1-9A20-8915A09A2BCE}" name="Table1" displayName="Table1" ref="A1:D36" totalsRowShown="0">
+  <autoFilter ref="A1:D36" xr:uid="{071852ED-39C9-45C1-9A20-8915A09A2BCE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{62508B5C-3DDE-4E48-BF30-EA74293F0000}" name="#"/>
+    <tableColumn id="2" xr3:uid="{DECC0C0D-F9D3-4429-8173-EA2CDED13AF6}" name="View"/>
+    <tableColumn id="3" xr3:uid="{D2EA0324-7F52-4037-8645-7615B82F5804}" name="Module"/>
+    <tableColumn id="4" xr3:uid="{8ACE2BE0-2729-4867-9278-54D61AE6BF21}" name="Model"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2022,21 +2187,21 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16.5">
+    <row r="22" spans="1:4">
       <c r="A22" s="12"/>
     </row>
-    <row r="23" spans="1:4" ht="16.5">
+    <row r="23" spans="1:4">
       <c r="A23" s="12"/>
     </row>
-    <row r="24" spans="1:4" ht="16.5">
+    <row r="24" spans="1:4">
       <c r="A24" s="12"/>
     </row>
-    <row r="25" spans="1:4" ht="16.5">
+    <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16.5">
+    <row r="26" spans="1:4">
       <c r="A26" s="12" t="s">
         <v>78</v>
       </c>
@@ -2044,7 +2209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5">
+    <row r="27" spans="1:4">
       <c r="A27" s="12" t="s">
         <v>79</v>
       </c>
@@ -2052,10 +2217,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.5">
+    <row r="28" spans="1:4">
       <c r="A28" s="12"/>
     </row>
-    <row r="29" spans="1:4" ht="16.5">
+    <row r="29" spans="1:4">
       <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>81</v>
@@ -2067,25 +2232,25 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16.5">
+    <row r="30" spans="1:4">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.5">
+    <row r="31" spans="1:4">
       <c r="A31" s="12"/>
     </row>
-    <row r="32" spans="1:4" ht="16.5">
+    <row r="32" spans="1:4">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:1" ht="16.5">
+    <row r="33" spans="1:1">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:1" ht="16.5">
+    <row r="34" spans="1:1">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:1" ht="16.5">
+    <row r="35" spans="1:1">
       <c r="A35" s="12"/>
     </row>
     <row r="36" spans="1:1">
@@ -2124,7 +2289,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:16" ht="16.5">
+    <row r="2" spans="1:16">
       <c r="A2" s="12" t="s">
         <v>84</v>
       </c>
@@ -2132,7 +2297,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.5">
+    <row r="3" spans="1:16">
       <c r="A3" s="12" t="s">
         <v>85</v>
       </c>
@@ -2148,7 +2313,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.5">
+    <row r="5" spans="1:16">
       <c r="A5" s="12" t="s">
         <v>87</v>
       </c>
@@ -2156,7 +2321,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5">
+    <row r="6" spans="1:16">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -2164,7 +2329,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16.5">
+    <row r="7" spans="1:16">
       <c r="A7" s="12" t="s">
         <v>89</v>
       </c>
@@ -2175,7 +2340,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5">
+    <row r="8" spans="1:16">
       <c r="A8" s="12" t="s">
         <v>90</v>
       </c>
@@ -2186,7 +2351,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16.5">
+    <row r="9" spans="1:16">
       <c r="A9" s="12" t="s">
         <v>91</v>
       </c>
@@ -2197,7 +2362,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.5">
+    <row r="10" spans="1:16">
       <c r="A10" s="12" t="s">
         <v>89</v>
       </c>
@@ -2208,7 +2373,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16.5">
+    <row r="11" spans="1:16">
       <c r="A11" s="12" t="s">
         <v>92</v>
       </c>
@@ -2219,7 +2384,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16.5">
+    <row r="12" spans="1:16">
       <c r="A12" s="12" t="s">
         <v>93</v>
       </c>
@@ -2230,7 +2395,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16.5">
+    <row r="13" spans="1:16">
       <c r="A13" s="12" t="s">
         <v>89</v>
       </c>
@@ -2241,7 +2406,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.5">
+    <row r="14" spans="1:16">
       <c r="A14" s="12" t="s">
         <v>94</v>
       </c>
@@ -2252,7 +2417,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16.5">
+    <row r="15" spans="1:16">
       <c r="A15" s="12" t="s">
         <v>95</v>
       </c>
@@ -2263,7 +2428,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16.5">
+    <row r="16" spans="1:16">
       <c r="A16" s="12" t="s">
         <v>96</v>
       </c>
@@ -2285,7 +2450,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="16.5">
+    <row r="18" spans="1:16">
       <c r="A18" s="12" t="s">
         <v>98</v>
       </c>
@@ -2296,7 +2461,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="16.5">
+    <row r="19" spans="1:16">
       <c r="A19" s="12" t="s">
         <v>99</v>
       </c>
@@ -2307,7 +2472,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="16.5">
+    <row r="20" spans="1:16">
       <c r="A20" s="12" t="s">
         <v>100</v>
       </c>
@@ -2315,7 +2480,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="16.5">
+    <row r="21" spans="1:16">
       <c r="A21" s="12" t="s">
         <v>101</v>
       </c>
@@ -2323,7 +2488,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="16.5">
+    <row r="22" spans="1:16">
       <c r="A22" s="12" t="s">
         <v>102</v>
       </c>
@@ -2331,7 +2496,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="16.5">
+    <row r="23" spans="1:16">
       <c r="A23" s="12" t="s">
         <v>103</v>
       </c>
@@ -2339,7 +2504,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="16.5">
+    <row r="24" spans="1:16">
       <c r="A24" s="12" t="s">
         <v>104</v>
       </c>
@@ -2347,17 +2512,17 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="16.5">
+    <row r="25" spans="1:16">
       <c r="P25" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="16.5">
+    <row r="26" spans="1:16">
       <c r="P26" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="16.5">
+    <row r="27" spans="1:16">
       <c r="P27" s="12" t="s">
         <v>132</v>
       </c>
@@ -2371,7 +2536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38477F8-6359-40BD-9417-44E5736CB004}">
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -2453,4 +2618,524 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0901BC3D-CC12-48EE-8FD2-4D03B317AF5C}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D35FC9F8-887C-4877-AAD7-4967BDEBF4E2}">
+          <x14:formula1>
+            <xm:f>Options!$A$3:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D36</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{611F8404-243E-4AAB-B4C5-E83E62DDE55F}">
+          <x14:formula1>
+            <xm:f>Options!$B$3:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C36</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79A533C-5919-4F8B-9661-41B3722978B9}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A1:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="91.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8253E9B4-BF1C-4659-8268-01A6809565AF}">
+  <dimension ref="A2:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on new design for the project
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\api\hud\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D1A0C-0710-475B-9FA8-9E0F73DCB766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650F7079-A59A-448B-889B-A1DB8DF1F2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26715" windowHeight="15315" activeTab="4" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="218">
   <si>
     <t>add item form</t>
   </si>
@@ -624,12 +624,108 @@
   <si>
     <t>get_document_dict</t>
   </si>
+  <si>
+    <t>mgt_home</t>
+  </si>
+  <si>
+    <t>mgt_stocks</t>
+  </si>
+  <si>
+    <t>mgt_users</t>
+  </si>
+  <si>
+    <t>mgt_update_permissions</t>
+  </si>
+  <si>
+    <t>mgt_update_group_permissions</t>
+  </si>
+  <si>
+    <t>add_product</t>
+  </si>
+  <si>
+    <t>mgt_price_tags</t>
+  </si>
+  <si>
+    <t>mgt_invoice_template_view</t>
+  </si>
+  <si>
+    <t>mgt_price_tags_control</t>
+  </si>
+  <si>
+    <t>product_datatable_view</t>
+  </si>
+  <si>
+    <t>documents_datatable_view</t>
+  </si>
+  <si>
+    <t>document_items_datatable_view</t>
+  </si>
+  <si>
+    <t>mgt_orders</t>
+  </si>
+  <si>
+    <t>modal_add_group</t>
+  </si>
+  <si>
+    <t>modal_add_user</t>
+  </si>
+  <si>
+    <t>add_new_order_tab</t>
+  </si>
+  <si>
+    <t>update_product_group</t>
+  </si>
+  <si>
+    <t>add_product_group</t>
+  </si>
+  <si>
+    <t>delete_product</t>
+  </si>
+  <si>
+    <t>delete_product_group</t>
+  </si>
+  <si>
+    <t>mgt_price_tags_preview</t>
+  </si>
+  <si>
+    <t>mgt_price_tags_set_default</t>
+  </si>
+  <si>
+    <t>mgt_price_tags_print_selected</t>
+  </si>
+  <si>
+    <t>mgt_export_products_to_csv</t>
+  </si>
+  <si>
+    <t>mgt_export_products_to_excel</t>
+  </si>
+  <si>
+    <t>add_doc_filter_products</t>
+  </si>
+  <si>
+    <t>management_views</t>
+  </si>
+  <si>
+    <t>stock_manager_views</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Aaccounts</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,8 +890,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{071852ED-39C9-45C1-9A20-8915A09A2BCE}" name="Table1" displayName="Table1" ref="A1:D36" totalsRowShown="0">
-  <autoFilter ref="A1:D36" xr:uid="{071852ED-39C9-45C1-9A20-8915A09A2BCE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{071852ED-39C9-45C1-9A20-8915A09A2BCE}" name="Table1" displayName="Table1" ref="A1:D61" totalsRowShown="0">
+  <autoFilter ref="A1:D61" xr:uid="{071852ED-39C9-45C1-9A20-8915A09A2BCE}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{62508B5C-3DDE-4E48-BF30-EA74293F0000}" name="#"/>
     <tableColumn id="2" xr3:uid="{DECC0C0D-F9D3-4429-8173-EA2CDED13AF6}" name="View"/>
@@ -1129,7 +1225,7 @@
       <selection activeCell="C38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -1144,7 +1240,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:10">
+    <row r="1" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="6:10">
+    <row r="2" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>1</v>
       </c>
@@ -1169,7 +1265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="6:10">
+    <row r="3" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F3">
         <v>2</v>
       </c>
@@ -1177,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="6:10">
+    <row r="4" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>3</v>
       </c>
@@ -1185,7 +1281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="6:10">
+    <row r="5" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>4</v>
       </c>
@@ -1199,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="6:10">
+    <row r="6" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>5</v>
       </c>
@@ -1213,12 +1309,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="6:10">
+    <row r="10" spans="6:10" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="6:10">
+    <row r="12" spans="6:10" x14ac:dyDescent="0.25">
       <c r="G12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1232,27 +1328,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="6:10">
+    <row r="13" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="6:10">
+    <row r="14" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="6:10">
+    <row r="15" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="6:10">
+    <row r="16" spans="6:10" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1266,7 +1362,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1302,7 +1398,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1372,7 +1468,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1406,7 +1502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1443,7 +1539,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1477,7 +1573,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1511,7 +1607,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1545,7 +1641,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1579,7 +1675,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1613,7 +1709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1641,7 +1737,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1660,7 +1756,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1679,27 +1775,27 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="60">
+    <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="K34" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K35" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K36" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K37" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30">
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="K38" s="7" t="s">
         <v>59</v>
       </c>
@@ -1717,7 +1813,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -1732,7 +1828,7 @@
     <col min="12" max="12" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1746,7 +1842,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1782,7 +1878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1818,7 +1914,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1852,7 +1948,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1888,7 +1984,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1925,7 +2021,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1959,7 +2055,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -1995,7 +2091,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2031,7 +2127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -2065,7 +2161,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -2099,7 +2195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2129,7 +2225,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2148,7 +2244,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -2167,41 +2263,41 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>78</v>
       </c>
@@ -2209,7 +2305,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>79</v>
       </c>
@@ -2217,10 +2313,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>81</v>
@@ -2232,46 +2328,46 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="D30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
     </row>
   </sheetData>
@@ -2287,9 +2383,9 @@
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>84</v>
       </c>
@@ -2297,7 +2393,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>85</v>
       </c>
@@ -2305,7 +2401,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>86</v>
       </c>
@@ -2313,7 +2409,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>87</v>
       </c>
@@ -2321,7 +2417,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>88</v>
       </c>
@@ -2329,7 +2425,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>89</v>
       </c>
@@ -2340,7 +2436,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>90</v>
       </c>
@@ -2351,7 +2447,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>91</v>
       </c>
@@ -2362,7 +2458,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>89</v>
       </c>
@@ -2373,7 +2469,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>92</v>
       </c>
@@ -2384,7 +2480,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>93</v>
       </c>
@@ -2395,7 +2491,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>89</v>
       </c>
@@ -2406,7 +2502,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>94</v>
       </c>
@@ -2417,7 +2513,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>95</v>
       </c>
@@ -2428,7 +2524,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>96</v>
       </c>
@@ -2439,7 +2535,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>97</v>
       </c>
@@ -2450,7 +2546,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>98</v>
       </c>
@@ -2461,7 +2557,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>99</v>
       </c>
@@ -2472,7 +2568,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>100</v>
       </c>
@@ -2480,7 +2576,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>101</v>
       </c>
@@ -2488,7 +2584,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>102</v>
       </c>
@@ -2496,7 +2592,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>103</v>
       </c>
@@ -2504,7 +2600,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>104</v>
       </c>
@@ -2512,17 +2608,17 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="P25" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="P26" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="P27" s="12" t="s">
         <v>132</v>
       </c>
@@ -2540,17 +2636,17 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>37</v>
       </c>
@@ -2558,7 +2654,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>37</v>
       </c>
@@ -2566,7 +2662,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>37</v>
       </c>
@@ -2574,43 +2670,43 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="13"/>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>39</v>
       </c>
@@ -2622,20 +2718,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0901BC3D-CC12-48EE-8FD2-4D03B317AF5C}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18:N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="29.28515625" customWidth="1"/>
+    <col min="14" max="14" width="35.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -2649,26 +2752,50 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="I2" t="s">
+        <v>186</v>
+      </c>
+      <c r="K2" t="s">
+        <v>214</v>
+      </c>
+      <c r="L2" t="s">
+        <v>217</v>
+      </c>
+      <c r="M2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>149</v>
+      </c>
+      <c r="P2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
         <v>147</v>
@@ -2676,13 +2803,34 @@
       <c r="D3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="I3" t="s">
+        <v>187</v>
+      </c>
+      <c r="K3" t="s">
+        <v>186</v>
+      </c>
+      <c r="L3" t="s">
+        <v>198</v>
+      </c>
+      <c r="M3" t="s">
+        <v>191</v>
+      </c>
+      <c r="N3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O3" t="s">
+        <v>187</v>
+      </c>
+      <c r="P3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -2690,279 +2838,791 @@
       <c r="D4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="I4" t="s">
+        <v>188</v>
+      </c>
+      <c r="L4" t="s">
+        <v>177</v>
+      </c>
+      <c r="M4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" t="s">
+        <v>178</v>
+      </c>
+      <c r="P4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="I5" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" t="s">
+        <v>201</v>
+      </c>
+      <c r="M5" t="s">
+        <v>192</v>
+      </c>
+      <c r="N5" t="s">
+        <v>196</v>
+      </c>
+      <c r="P5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="I6" t="s">
+        <v>190</v>
+      </c>
+      <c r="M6" t="s">
+        <v>193</v>
+      </c>
+      <c r="N6" t="s">
+        <v>181</v>
+      </c>
+      <c r="P6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>159</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="I7" t="s">
+        <v>191</v>
+      </c>
+      <c r="M7" t="s">
+        <v>194</v>
+      </c>
+      <c r="N7" t="s">
+        <v>169</v>
+      </c>
+      <c r="P7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>160</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="M8" t="s">
+        <v>195</v>
+      </c>
+      <c r="N8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="N9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="D10" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="M10" t="s">
+        <v>199</v>
+      </c>
+      <c r="N10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="I11" t="s">
+        <v>192</v>
+      </c>
+      <c r="M11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="I12" t="s">
+        <v>192</v>
+      </c>
+      <c r="M12" t="s">
+        <v>159</v>
+      </c>
+      <c r="N12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13" t="s">
+        <v>193</v>
+      </c>
+      <c r="M13" t="s">
+        <v>158</v>
+      </c>
+      <c r="N13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14" t="s">
+        <v>194</v>
+      </c>
+      <c r="I14" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>195</v>
+      </c>
+      <c r="I15" t="s">
+        <v>195</v>
+      </c>
+      <c r="M15" t="s">
+        <v>160</v>
+      </c>
+      <c r="N15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>152</v>
+      </c>
+      <c r="I16" t="s">
+        <v>152</v>
+      </c>
+      <c r="M16" t="s">
+        <v>164</v>
+      </c>
+      <c r="N16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>178</v>
+      </c>
+      <c r="I17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>175</v>
+      </c>
+      <c r="I18" t="s">
+        <v>175</v>
+      </c>
+      <c r="M18" t="s">
+        <v>202</v>
+      </c>
+      <c r="N18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>196</v>
+      </c>
+      <c r="I19" t="s">
+        <v>196</v>
+      </c>
+      <c r="M19" t="s">
+        <v>203</v>
+      </c>
+      <c r="N19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>181</v>
+      </c>
+      <c r="I20" t="s">
+        <v>181</v>
+      </c>
+      <c r="M20" t="s">
+        <v>204</v>
+      </c>
+      <c r="N20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>169</v>
+      </c>
+      <c r="I21" t="s">
+        <v>169</v>
+      </c>
+      <c r="M21" t="s">
+        <v>205</v>
+      </c>
+      <c r="N21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>182</v>
+      </c>
+      <c r="I22" t="s">
+        <v>182</v>
+      </c>
+      <c r="N22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>183</v>
+      </c>
+      <c r="I23" t="s">
+        <v>183</v>
+      </c>
+      <c r="M23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>197</v>
+      </c>
+      <c r="I24" t="s">
+        <v>197</v>
+      </c>
+      <c r="M24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="I25" t="s">
+        <v>175</v>
+      </c>
+      <c r="M25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>198</v>
+      </c>
+      <c r="I26" t="s">
+        <v>198</v>
+      </c>
+      <c r="M26" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>177</v>
+      </c>
+      <c r="I27" t="s">
+        <v>177</v>
+      </c>
+      <c r="M27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>199</v>
+      </c>
+      <c r="I28" t="s">
+        <v>199</v>
+      </c>
+      <c r="M28" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>200</v>
+      </c>
+      <c r="I29" t="s">
+        <v>200</v>
+      </c>
+      <c r="M29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>154</v>
+      </c>
+      <c r="I30" t="s">
+        <v>154</v>
+      </c>
+      <c r="M30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>166</v>
+      </c>
+      <c r="I31" t="s">
+        <v>166</v>
+      </c>
+      <c r="M31" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>165</v>
+      </c>
+      <c r="I32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>154</v>
+      </c>
+      <c r="I33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>159</v>
+      </c>
+      <c r="I34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>158</v>
+      </c>
+      <c r="I35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>185</v>
+        <v>157</v>
+      </c>
+      <c r="I36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>160</v>
+      </c>
+      <c r="I37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>164</v>
+      </c>
+      <c r="I38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>167</v>
+      </c>
+      <c r="I39" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>201</v>
+      </c>
+      <c r="I40" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>171</v>
+      </c>
+      <c r="I41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>170</v>
+      </c>
+      <c r="I42" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>202</v>
+      </c>
+      <c r="I43" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>203</v>
+      </c>
+      <c r="I44" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>204</v>
+      </c>
+      <c r="I45" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>205</v>
+      </c>
+      <c r="I46" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>161</v>
+      </c>
+      <c r="I47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>162</v>
+      </c>
+      <c r="I48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>163</v>
+      </c>
+      <c r="I49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>155</v>
+      </c>
+      <c r="I50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>156</v>
+      </c>
+      <c r="I51" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>206</v>
+      </c>
+      <c r="I52" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>207</v>
+      </c>
+      <c r="I53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>208</v>
+      </c>
+      <c r="I54" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>209</v>
+      </c>
+      <c r="I55" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>210</v>
+      </c>
+      <c r="I56" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>168</v>
+      </c>
+      <c r="I57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>211</v>
+      </c>
+      <c r="I58" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>184</v>
+      </c>
+      <c r="I59" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>174</v>
+      </c>
+      <c r="I60" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>173</v>
+      </c>
+      <c r="I61" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2972,18 +3632,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D35FC9F8-887C-4877-AAD7-4967BDEBF4E2}">
           <x14:formula1>
             <xm:f>Options!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D36</xm:sqref>
+          <xm:sqref>D2:D61</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{611F8404-243E-4AAB-B4C5-E83E62DDE55F}">
           <x14:formula1>
             <xm:f>Options!$B$3:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C36</xm:sqref>
+          <xm:sqref>C3:C61</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6FBB2246-7455-4F69-8E8F-5EC96B9BFBE9}">
+          <x14:formula1>
+            <xm:f>Options!$B$3:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2999,82 +3665,82 @@
       <selection activeCell="A15" sqref="A1:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="91.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>185</v>
       </c>
@@ -3086,19 +3752,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8253E9B4-BF1C-4659-8268-01A6809565AF}">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -3106,7 +3772,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -3114,7 +3780,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3122,7 +3788,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -3130,9 +3796,19 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on a new layout for the sysstem
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650F7079-A59A-448B-889B-A1DB8DF1F2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12047E17-9F72-4591-A5F5-C3325450CF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="order_item" sheetId="3" r:id="rId3"/>
     <sheet name="Tree" sheetId="4" r:id="rId4"/>
     <sheet name="Views" sheetId="5" r:id="rId5"/>
-    <sheet name="temp" sheetId="7" r:id="rId6"/>
+    <sheet name="components" sheetId="7" r:id="rId6"/>
     <sheet name="Options" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="242">
   <si>
     <t>add item form</t>
   </si>
@@ -583,9 +583,6 @@
     <t>add_new_document_edit_item</t>
   </si>
   <si>
-    <t>DocumentSerializer</t>
-  </si>
-  <si>
     <t>ItemListView</t>
   </si>
   <si>
@@ -595,21 +592,12 @@
     <t>mgt_documents_example</t>
   </si>
   <si>
-    <t>create_order_dict</t>
-  </si>
-  <si>
     <t>mgt_add_new_order</t>
   </si>
   <si>
     <t>add_document</t>
   </si>
   <si>
-    <t>documents_datatable_view2</t>
-  </si>
-  <si>
-    <t>mgt_documents2</t>
-  </si>
-  <si>
     <t>add_document_items_to_document</t>
   </si>
   <si>
@@ -622,9 +610,6 @@
     <t>DocumentListView</t>
   </si>
   <si>
-    <t>get_document_dict</t>
-  </si>
-  <si>
     <t>mgt_home</t>
   </si>
   <si>
@@ -719,13 +704,100 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>Product List</t>
+  </si>
+  <si>
+    <t>Product Item</t>
+  </si>
+  <si>
+    <t>Order List</t>
+  </si>
+  <si>
+    <t>Order Item</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Search Products</t>
+  </si>
+  <si>
+    <t>filter by caategories</t>
+  </si>
+  <si>
+    <t>Customer | name, details</t>
+  </si>
+  <si>
+    <t>Pages</t>
+  </si>
+  <si>
+    <t>1. POS</t>
+  </si>
+  <si>
+    <t>Home screen</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>- list</t>
+  </si>
+  <si>
+    <t>- Add new product</t>
+  </si>
+  <si>
+    <t>- Edit product</t>
+  </si>
+  <si>
+    <t>- Delete Product</t>
+  </si>
+  <si>
+    <t>- Filter product by category</t>
+  </si>
+  <si>
+    <t>- Add product group</t>
+  </si>
+  <si>
+    <t>- Edit group</t>
+  </si>
+  <si>
+    <t>- Delete group</t>
+  </si>
+  <si>
+    <t>- Export list</t>
+  </si>
+  <si>
+    <t>- Price tags</t>
+  </si>
+  <si>
+    <t>- Sorting</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>RS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,8 +836,31 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Wingdings 2"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -808,6 +903,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -841,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -872,11 +973,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2720,7 +2856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0901BC3D-CC12-48EE-8FD2-4D03B317AF5C}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N18" sqref="N18:N22"/>
     </sheetView>
   </sheetViews>
@@ -2757,22 +2893,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D2" t="s">
         <v>146</v>
       </c>
       <c r="I2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="K2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="L2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="M2" t="s">
         <v>146</v>
@@ -2784,10 +2920,10 @@
         <v>149</v>
       </c>
       <c r="P2" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="Q2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2795,7 +2931,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
         <v>147</v>
@@ -2804,25 +2940,25 @@
         <v>146</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L3" t="s">
+        <v>193</v>
+      </c>
+      <c r="M3" t="s">
         <v>186</v>
-      </c>
-      <c r="L3" t="s">
-        <v>198</v>
-      </c>
-      <c r="M3" t="s">
-        <v>191</v>
       </c>
       <c r="N3" t="s">
         <v>152</v>
       </c>
       <c r="O3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="P3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -2830,7 +2966,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
         <v>151</v>
@@ -2839,19 +2975,19 @@
         <v>146</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="L4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M4" t="s">
         <v>147</v>
       </c>
       <c r="N4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="P4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2859,25 +2995,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D5" t="s">
         <v>146</v>
       </c>
       <c r="I5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="L5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="M5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="N5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="P5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -2885,22 +3021,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
         <v>146</v>
       </c>
       <c r="I6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="M6" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="N6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="P6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2908,16 +3044,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
         <v>146</v>
       </c>
       <c r="I7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="M7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="N7" t="s">
         <v>169</v>
@@ -2931,16 +3067,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
         <v>146</v>
       </c>
       <c r="M8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="N8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2954,7 +3090,7 @@
         <v>146</v>
       </c>
       <c r="N9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2968,10 +3104,10 @@
         <v>146</v>
       </c>
       <c r="M10" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="N10" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -2979,13 +3115,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D11" t="s">
         <v>146</v>
       </c>
       <c r="I11" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M11" t="s">
         <v>154</v>
@@ -2996,13 +3132,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D12" t="s">
         <v>146</v>
       </c>
       <c r="I12" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="M12" t="s">
         <v>159</v>
@@ -3016,10 +3152,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="I13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="M13" t="s">
         <v>158</v>
@@ -3033,10 +3169,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="M14" t="s">
         <v>157</v>
@@ -3047,10 +3183,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I15" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="M15" t="s">
         <v>160</v>
@@ -3081,10 +3217,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3092,13 +3228,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M18" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="N18" t="s">
         <v>168</v>
@@ -3109,16 +3245,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I19" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M19" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N19" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -3126,16 +3262,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I20" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="M20" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="N20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3149,10 +3285,10 @@
         <v>169</v>
       </c>
       <c r="M21" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="N21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -3160,13 +3296,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I22" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="N22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -3174,10 +3310,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I23" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M23" t="s">
         <v>162</v>
@@ -3188,10 +3324,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I24" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="M24" t="s">
         <v>163</v>
@@ -3202,10 +3338,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M25" t="s">
         <v>155</v>
@@ -3216,10 +3352,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I26" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="M26" t="s">
         <v>156</v>
@@ -3230,13 +3366,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M27" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -3244,13 +3380,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I28" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="M28" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -3258,13 +3394,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="I29" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="M29" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3278,7 +3414,7 @@
         <v>154</v>
       </c>
       <c r="M30" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -3292,7 +3428,7 @@
         <v>166</v>
       </c>
       <c r="M31" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -3388,10 +3524,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I40" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3421,10 +3557,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="I43" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3432,10 +3568,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I44" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3443,10 +3579,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I45" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3454,10 +3590,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I46" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3520,10 +3656,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I52" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3531,10 +3667,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I53" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3542,10 +3678,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I54" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3553,10 +3689,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I55" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3564,10 +3700,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I56" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3586,10 +3722,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I58" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3597,10 +3733,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I59" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3608,10 +3744,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3619,10 +3755,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3659,93 +3795,1212 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79A533C-5919-4F8B-9661-41B3722978B9}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A1:A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="91.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="20" t="str">
+        <f>IF(B2="t","R","S")</f>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="20" t="str">
+        <f t="shared" ref="C3:C66" si="0">IF(B3="t","R","S")</f>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>R</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>185</v>
+        <v>224</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C37" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C38" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C39" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C40" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C41" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C42" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C43" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C45" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C46" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C47" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C48" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C49" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C50" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C51" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C52" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C53" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C54" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C55" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C56" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C57" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C58" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C59" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C60" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C61" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C62" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C63" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C64" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C65" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C66" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C67" s="20" t="str">
+        <f t="shared" ref="C67:C130" si="1">IF(B67="t","R","S")</f>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C68" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C69" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C70" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C71" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C72" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C73" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C74" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C75" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C76" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C77" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C78" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C79" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C80" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C81" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C82" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C83" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C84" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C85" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C86" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C87" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C88" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C89" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C90" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C91" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C92" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C93" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C94" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C95" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C96" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C97" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C98" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C99" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C100" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C101" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C102" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C103" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C104" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C105" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C106" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C107" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C108" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C109" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C110" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C111" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C112" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C113" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C114" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C115" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C116" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C117" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C118" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C119" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C120" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C121" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C122" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C123" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C124" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C125" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C126" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C127" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C128" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C129" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C130" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C131" s="20" t="str">
+        <f t="shared" ref="C131:C173" si="2">IF(B131="t","R","S")</f>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C132" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C133" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C134" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C135" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C136" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C137" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C138" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C139" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C140" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C141" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C142" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C143" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C144" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C145" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C146" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C147" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C148" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C149" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C150" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C151" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C152" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C153" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="154" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C154" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C155" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C156" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C157" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C158" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C159" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="160" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C160" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C161" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C162" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C163" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C164" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C165" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C166" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C167" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C168" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C169" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C170" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C171" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C172" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="C173" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>S</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C173">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3803,12 +5058,12 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pin code input installed
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12047E17-9F72-4591-A5F5-C3325450CF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8413A214-231E-471A-9AFB-BA12415D206F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Tree" sheetId="4" r:id="rId4"/>
     <sheet name="Views" sheetId="5" r:id="rId5"/>
     <sheet name="components" sheetId="7" r:id="rId6"/>
-    <sheet name="Options" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="Options" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="248">
   <si>
     <t>add item form</t>
   </si>
@@ -791,6 +792,24 @@
   </si>
   <si>
     <t>RS</t>
+  </si>
+  <si>
+    <t>Airport</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Functionalities</t>
+  </si>
+  <si>
+    <t>Takeover user</t>
+  </si>
+  <si>
+    <t>Temporary user</t>
+  </si>
+  <si>
+    <t>Unlock with pasword</t>
   </si>
 </sst>
 </file>
@@ -984,7 +1003,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -999,16 +1018,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3797,7 +3806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79A533C-5919-4F8B-9661-41B3722978B9}">
   <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -4994,11 +5003,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C173">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"R"</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5006,20 +5015,70 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8253E9B4-BF1C-4659-8268-01A6809565AF}">
-  <dimension ref="A2:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C09989DC-20BE-427C-B52F-92180AC69020}">
+  <dimension ref="D5:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>800000</v>
+      </c>
+      <c r="E6">
+        <v>1484</v>
+      </c>
+      <c r="F6">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>404</v>
+      </c>
+      <c r="F7">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8253E9B4-BF1C-4659-8268-01A6809565AF}">
+  <dimension ref="A2:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>148</v>
       </c>
@@ -5027,7 +5086,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -5035,7 +5094,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -5043,7 +5102,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -5051,19 +5110,101 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>22250</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>114000</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>16500</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f>SUM(D12:D22)</f>
+        <v>264250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on the orders templates for pos
</commit_message>
<xml_diff>
--- a/docs/ad_new_document_form.xlsx
+++ b/docs/ad_new_document_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\api\hud\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8413A214-231E-471A-9AFB-BA12415D206F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1197548-A454-4559-9676-6F7A0A3DCF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{33FD871D-92BE-4C86-AA76-A6BD2228683F}"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="components" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
     <sheet name="Options" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="268">
   <si>
     <t>add item form</t>
   </si>
@@ -810,6 +811,66 @@
   </si>
   <si>
     <t>Unlock with pasword</t>
+  </si>
+  <si>
+    <t>Orders</t>
+  </si>
+  <si>
+    <t>items_list</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>calculations</t>
+  </si>
+  <si>
+    <t>order-details</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>visual</t>
+  </si>
+  <si>
+    <t>product_list</t>
+  </si>
+  <si>
+    <t>product_card</t>
+  </si>
+  <si>
+    <t>active_order</t>
+  </si>
+  <si>
+    <t>buttons</t>
+  </si>
+  <si>
+    <t>top_buttons</t>
+  </si>
+  <si>
+    <t>Barcodes</t>
+  </si>
+  <si>
+    <t>Barcode_input</t>
+  </si>
+  <si>
+    <t>input_buttons</t>
+  </si>
+  <si>
+    <t>payments</t>
+  </si>
+  <si>
+    <t>payment_modal</t>
+  </si>
+  <si>
+    <t>payment_types</t>
+  </si>
+  <si>
+    <t>calculator</t>
+  </si>
+  <si>
+    <t>paid_input</t>
   </si>
 </sst>
 </file>
@@ -2775,15 +2836,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38477F8-6359-40BD-9417-44E5736CB004}">
-  <dimension ref="B2:C14"/>
+  <dimension ref="A2:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -2854,6 +2916,147 @@
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>248</v>
+      </c>
+      <c r="C21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>250</v>
+      </c>
+      <c r="D22" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>251</v>
+      </c>
+      <c r="D23" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D24" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>257</v>
+      </c>
+      <c r="D26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>250</v>
+      </c>
+      <c r="D28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>251</v>
+      </c>
+      <c r="D29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>258</v>
+      </c>
+      <c r="C30" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>224</v>
+      </c>
+      <c r="C35" t="s">
+        <v>255</v>
+      </c>
+      <c r="D35" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>256</v>
+      </c>
+      <c r="D36" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>260</v>
+      </c>
+      <c r="C40" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>263</v>
+      </c>
+      <c r="C46" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -5068,7 +5271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8253E9B4-BF1C-4659-8268-01A6809565AF}">
   <dimension ref="A2:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -5210,4 +5413,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E78ED5A-4F74-49A7-9F69-1A33DB751621}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>